<commit_message>
added new countries list
</commit_message>
<xml_diff>
--- a/src/test/resources/Vytrack testusers.xlsx
+++ b/src/test/resources/Vytrack testusers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marufjon/IdeaProjects/fall-2019-selenium-project/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADCD3B5-D4BC-184A-85E6-D7CDF897C258}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B390D0F7-A610-AE4C-BF2F-5F39B0E519E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41060" yWindow="1000" windowWidth="33600" windowHeight="18920" activeTab="5" xr2:uid="{506372D9-39D2-EA47-AA3D-ABD5428ED2AB}"/>
   </bookViews>
@@ -4516,6 +4516,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F38E2B0C-F437-2D4A-858E-BB81DDD301FF}" name="Table1" displayName="Table1" ref="A1:E16" totalsRowShown="0">
+  <autoFilter ref="A1:E16" xr:uid="{3A1BC1BA-FF7F-7245-87DD-CE8144B1B2C2}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{FB8C5F0F-6F9B-7940-A189-6B06F33EE7B6}" name="username"/>
+    <tableColumn id="2" xr3:uid="{3490A29C-15DE-884E-A83B-326ED395E9A6}" name="password"/>
+    <tableColumn id="3" xr3:uid="{E3248777-7789-C542-9291-3E5D92F904D5}" name="firstname"/>
+    <tableColumn id="4" xr3:uid="{8D563738-FEB8-A64A-881E-D8B91833252A}" name="lastname"/>
+    <tableColumn id="5" xr3:uid="{8F560D2B-14F9-094C-B8FA-E38CE8312DAA}" name="result"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18234,7 +18248,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="226" zoomScaleNormal="226" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18518,5 +18532,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>